<commit_message>
graphing closer to working
</commit_message>
<xml_diff>
--- a/data/ihme-gbd.xlsx
+++ b/data/ihme-gbd.xlsx
@@ -1859,8 +1859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D335"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A320" workbookViewId="0">
-      <selection activeCell="F334" sqref="F334"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1889,6 +1889,9 @@
       <c r="B2">
         <v>71538.760351200006</v>
       </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
       <c r="D2">
         <v>2793436.6702200002</v>
       </c>
@@ -2123,6 +2126,9 @@
       </c>
       <c r="B19">
         <v>141942.952854</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
       </c>
       <c r="D19">
         <v>1481594.17652</v>

</xml_diff>

<commit_message>
fixed bug with new data file
</commit_message>
<xml_diff>
--- a/data/ihme-gbd.xlsx
+++ b/data/ihme-gbd.xlsx
@@ -1042,12 +1042,6 @@
     <t>thislevel</t>
   </si>
   <si>
-    <t>fullcause</t>
-  </si>
-  <si>
-    <t>shortcause</t>
-  </si>
-  <si>
     <t>HIV/AIDS &amp; tuberculosis</t>
   </si>
   <si>
@@ -1055,6 +1049,12 @@
   </si>
   <si>
     <t>TEMP</t>
+  </si>
+  <si>
+    <t>cause</t>
+  </si>
+  <si>
+    <t>short</t>
   </si>
 </sst>
 </file>
@@ -1887,8 +1887,8 @@
   <dimension ref="A1:J335"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C138" sqref="C138"/>
+      <pane ySplit="1" topLeftCell="A311" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G324" sqref="G324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1914,10 +1914,10 @@
         <v>341</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>336</v>
@@ -3793,16 +3793,16 @@
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B135" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E135">
         <v>2</v>
       </c>
       <c r="F135" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G135" t="s">
         <v>226</v>

</xml_diff>

<commit_message>
version of afghanistan results sent
</commit_message>
<xml_diff>
--- a/data/ihme-gbd.xlsx
+++ b/data/ihme-gbd.xlsx
@@ -1890,8 +1890,8 @@
   <dimension ref="A1:K335"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G137" sqref="G137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
modified in some way
</commit_message>
<xml_diff>
--- a/data/ihme-gbd.xlsx
+++ b/data/ihme-gbd.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="345">
   <si>
     <t>HIV/AIDS resulting in other diseases</t>
   </si>
@@ -1040,15 +1040,6 @@
   </si>
   <si>
     <t>thislevel</t>
-  </si>
-  <si>
-    <t>HIV/AIDS &amp; tuberculosis</t>
-  </si>
-  <si>
-    <t>Communicable diseases</t>
-  </si>
-  <si>
-    <t>TEMP</t>
   </si>
   <si>
     <t>cause</t>
@@ -1890,19 +1881,20 @@
   <dimension ref="A1:K335"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G137" sqref="G137"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="2" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>337</v>
@@ -1920,10 +1912,10 @@
         <v>341</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>336</v>
@@ -4199,18 +4191,6 @@
     <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>1</v>
-      </c>
-      <c r="B135" t="s">
-        <v>343</v>
-      </c>
-      <c r="C135" t="s">
-        <v>344</v>
-      </c>
-      <c r="F135">
-        <v>2</v>
-      </c>
-      <c r="G135" t="s">
-        <v>342</v>
       </c>
       <c r="H135" t="s">
         <v>226</v>

</xml_diff>